<commit_message>
Add a study plan
</commit_message>
<xml_diff>
--- a/weekly time plan.xlsx
+++ b/weekly time plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangha\Documents\Github\r4ds-instructors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F4A613-BDB7-4E6A-A63C-61ECABD99A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241A856B-0BE9-4C53-AAFC-79CD829404F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{36754BCE-2DE6-4F8E-9663-DFB1C7423350}"/>
+    <workbookView xWindow="8025" yWindow="2610" windowWidth="15105" windowHeight="11490" xr2:uid="{36754BCE-2DE6-4F8E-9663-DFB1C7423350}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Week</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Chp. 3 Data visualisation</t>
   </si>
   <si>
-    <t>Prepare</t>
-  </si>
-  <si>
-    <t>Assignment</t>
-  </si>
-  <si>
     <t>Some ggplot examples. Build in dataset in R</t>
   </si>
   <si>
@@ -147,6 +141,36 @@
   </si>
   <si>
     <t>How to use git and ADO Repos</t>
+  </si>
+  <si>
+    <t>chp 9, 10, 11</t>
+  </si>
+  <si>
+    <t>chp 12, 13</t>
+  </si>
+  <si>
+    <t>chp 14, 15</t>
+  </si>
+  <si>
+    <t>chp 16</t>
+  </si>
+  <si>
+    <t>chp 17, 18, 19</t>
+  </si>
+  <si>
+    <t>chp 20 and 21</t>
+  </si>
+  <si>
+    <t>chp 27</t>
+  </si>
+  <si>
+    <t>Preparation need from instructor</t>
+  </si>
+  <si>
+    <t>Assignment to read</t>
+  </si>
+  <si>
+    <t>Happy Git for R (Optional)</t>
   </si>
 </sst>
 </file>
@@ -501,219 +525,243 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="31.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.23046875" customWidth="1"/>
-    <col min="5" max="5" width="19.3828125" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>